<commit_message>
Update Relatório 4 - Lab TCM I
</commit_message>
<xml_diff>
--- a/Lab. Mec Flu I/Relatório_5/dados.xlsx
+++ b/Lab. Mec Flu I/Relatório_5/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNESP\EngMec-UNESP\Lab. Mec Flu I\Relatório_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A893F5F-6AC2-4F87-A49D-1BEA22D8BAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07425C97-DF20-4B0A-90D9-D7E3C5F522EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26268" yWindow="2748" windowWidth="17280" windowHeight="9420" xr2:uid="{E421D476-4456-4EC3-903C-40AF8793AE2E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E421D476-4456-4EC3-903C-40AF8793AE2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB37EB21-ACB2-439B-B8E2-D7E0CDD27665}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +504,7 @@
         <v>1.57</v>
       </c>
       <c r="B9">
-        <v>2.57</v>
+        <v>2.37</v>
       </c>
       <c r="C9">
         <v>2.2000000000000002</v>
@@ -515,7 +515,7 @@
         <v>1.88</v>
       </c>
       <c r="B10">
-        <v>3.08</v>
+        <v>2.93</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -525,7 +525,7 @@
       <c r="A11">
         <v>1.19</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1.94</v>
       </c>
       <c r="C11">
@@ -587,6 +587,12 @@
       <c r="C16">
         <v>0.8</v>
       </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>